<commit_message>
Atualização na documentação, função de colocar comentario no post esta funcionando
</commit_message>
<xml_diff>
--- a/Documentação/Product backlogs.xlsx
+++ b/Documentação/Product backlogs.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="472" documentId="11_AD4D361C20488DEA4E38A0F40C5A5BD05ADEDD78" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EACEA9FE-4EC0-4D26-B628-2D4F24C19837}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -516,7 +516,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -554,19 +554,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1085,8 +1082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1170,10 +1167,10 @@
       <c r="J2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="14"/>
+      <c r="M2" s="16"/>
     </row>
     <row r="3" spans="1:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -1404,10 +1401,10 @@
         <v>Sprint 1</v>
       </c>
       <c r="J8" s="6"/>
-      <c r="L8" s="15" t="s">
+      <c r="L8" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="M8" s="16">
+      <c r="M8" s="14">
         <f>SUM(H:H)</f>
         <v>216</v>
       </c>
@@ -1892,11 +1889,11 @@
       <c r="G23" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="H23" s="17">
+      <c r="H23" s="6">
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>8</v>
       </c>
-      <c r="I23" s="17" t="str">
+      <c r="I23" s="6" t="str">
         <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
         <v>Sprint 1</v>
       </c>
@@ -1958,11 +1955,11 @@
       <c r="G25" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H25" s="17">
+      <c r="H25" s="6">
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>8</v>
       </c>
-      <c r="I25" s="17" t="str">
+      <c r="I25" s="6" t="str">
         <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
         <v>Sprint 1</v>
       </c>
@@ -1990,11 +1987,11 @@
       <c r="G26" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H26" s="17">
+      <c r="H26" s="6">
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>5</v>
       </c>
-      <c r="I26" s="17" t="str">
+      <c r="I26" s="6" t="str">
         <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
         <v>Sprint 1</v>
       </c>
@@ -2122,11 +2119,11 @@
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
-      <c r="H31" s="17" t="str">
+      <c r="H31" s="6" t="str">
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v/>
       </c>
-      <c r="I31" s="17" t="str">
+      <c r="I31" s="6" t="str">
         <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
         <v/>
       </c>
@@ -2140,11 +2137,11 @@
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
-      <c r="H32" s="17" t="str">
+      <c r="H32" s="6" t="str">
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v/>
       </c>
-      <c r="I32" s="17" t="str">
+      <c r="I32" s="6" t="str">
         <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
         <v/>
       </c>

</xml_diff>

<commit_message>
Atualização na documentação(marcos do projeto) e atualização no product backlogs
</commit_message>
<xml_diff>
--- a/Documentação/Product backlogs.xlsx
+++ b/Documentação/Product backlogs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/samuel_barros_sptech_school/Documents/Documentos/Algoritmo/Aula 3/SPtech/Projeto-pessoal/Documentação/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="472" documentId="11_AD4D361C20488DEA4E38A0F40C5A5BD05ADEDD78" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EACEA9FE-4EC0-4D26-B628-2D4F24C19837}"/>
+  <xr:revisionPtr revIDLastSave="496" documentId="11_AD4D361C20488DEA4E38A0F40C5A5BD05ADEDD78" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E700C25-CE6B-4BA5-BB1D-BD97477A45A8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="103">
   <si>
     <t>Categoria</t>
   </si>
@@ -161,9 +161,6 @@
     <t>Grande</t>
   </si>
   <si>
-    <t>No campo avistamento poderá ser colocado uma imagem em até 50 MB.</t>
-  </si>
-  <si>
     <t>Contas comuns terá acesso ao conteúdo padrão.</t>
   </si>
   <si>
@@ -278,9 +275,6 @@
     <t>No campo descrição será até 200 caracteres.</t>
   </si>
   <si>
-    <t>No campo relato poderá ser colocado um relato em até 300 caracteres.</t>
-  </si>
-  <si>
     <t>Site</t>
   </si>
   <si>
@@ -342,6 +336,15 @@
   </si>
   <si>
     <t>Muito pequeno</t>
+  </si>
+  <si>
+    <t>No campo avistamento poderá ser colocado uma imagem.</t>
+  </si>
+  <si>
+    <t>RF 10.2</t>
+  </si>
+  <si>
+    <t>RF 10.3</t>
   </si>
 </sst>
 </file>
@@ -516,7 +519,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -566,6 +569,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,6 +590,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -599,7 +606,6 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -795,8 +801,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{45B462BB-5B87-483D-98E3-29AB6CAFCDBD}" name="Tabela1" displayName="Tabela1" ref="A1:J32" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10">
-  <autoFilter ref="A1:J32" xr:uid="{45B462BB-5B87-483D-98E3-29AB6CAFCDBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{45B462BB-5B87-483D-98E3-29AB6CAFCDBD}" name="Tabela1" displayName="Tabela1" ref="A1:J28" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10">
+  <autoFilter ref="A1:J28" xr:uid="{45B462BB-5B87-483D-98E3-29AB6CAFCDBD}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{B1D35C00-40CB-4287-9052-ECF958F0F43F}" name="Categoria" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{EB622D7D-86A0-4DD4-8D1C-EFC82501F5A5}" name="Identificador" dataDxfId="8"/>
@@ -808,10 +814,10 @@
     <tableColumn id="8" xr3:uid="{E55713D6-BEF4-4E2B-A894-0176E4987129}" name="Tam(#)" dataDxfId="2">
       <calculatedColumnFormula>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{53EA01A0-EC01-402F-BA49-1E4B7904D7B8}" name="Sprint" dataDxfId="1">
-      <calculatedColumnFormula>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</calculatedColumnFormula>
+    <tableColumn id="9" xr3:uid="{53EA01A0-EC01-402F-BA49-1E4B7904D7B8}" name="Sprint" dataDxfId="0">
+      <calculatedColumnFormula>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{D68286FD-EF48-4F7F-B2D3-35D2D998121E}" name="Sprint semanal" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{D68286FD-EF48-4F7F-B2D3-35D2D998121E}" name="Sprint semanal" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1080,10 +1086,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1160,9 +1166,9 @@
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>5</v>
       </c>
-      <c r="I2" s="6" t="str">
-        <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
-        <v>Sprint 1</v>
+      <c r="I2" s="6">
+        <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
+        <v>5</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>14</v>
@@ -1177,7 +1183,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>21</v>
@@ -1198,16 +1204,16 @@
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>8</v>
       </c>
-      <c r="I3" s="6" t="str">
-        <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
-        <v>Sprint 1</v>
+      <c r="I3" s="6">
+        <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
+        <v>8</v>
       </c>
       <c r="J3" s="6"/>
       <c r="L3" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1215,7 +1221,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>16</v>
@@ -1236,9 +1242,9 @@
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>5</v>
       </c>
-      <c r="I4" s="6" t="str">
-        <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
-        <v>Sprint 1</v>
+      <c r="I4" s="6">
+        <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
+        <v>5</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>14</v>
@@ -1256,7 +1262,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>18</v>
@@ -1277,15 +1283,15 @@
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>5</v>
       </c>
-      <c r="I5" s="6" t="str">
-        <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
-        <v>Sprint 1</v>
+      <c r="I5" s="6">
+        <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
+        <v>5</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>14</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="M5" s="10">
         <f>SUMIF(J:J,"Semana 2",H:H)</f>
@@ -1297,13 +1303,13 @@
         <v>10</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>12</v>
@@ -1318,13 +1324,13 @@
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>8</v>
       </c>
-      <c r="I6" s="6" t="str">
-        <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
-        <v>Sprint 1</v>
+      <c r="I6" s="6">
+        <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
+        <v>8</v>
       </c>
       <c r="J6" s="6"/>
       <c r="L6" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M6" s="10">
         <f>SUMIF(J:J,"Semana 3",H:H)</f>
@@ -1336,13 +1342,13 @@
         <v>10</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>12</v>
@@ -1357,13 +1363,13 @@
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>8</v>
       </c>
-      <c r="I7" s="6" t="str">
-        <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
-        <v>Sprint 1</v>
+      <c r="I7" s="6">
+        <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
+        <v>8</v>
       </c>
       <c r="J7" s="6"/>
       <c r="L7" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M7" s="12">
         <f>SUMIF(J:J,"Semana 4",H:H)</f>
@@ -1375,13 +1381,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>12</v>
@@ -1396,17 +1402,17 @@
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>8</v>
       </c>
-      <c r="I8" s="6" t="str">
-        <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
-        <v>Sprint 1</v>
+      <c r="I8" s="6">
+        <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
+        <v>8</v>
       </c>
       <c r="J8" s="6"/>
       <c r="L8" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="M8" s="14">
         <f>SUM(H:H)</f>
-        <v>216</v>
+        <v>203</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1414,13 +1420,13 @@
         <v>10</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>12</v>
@@ -1435,9 +1441,9 @@
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>8</v>
       </c>
-      <c r="I9" s="6" t="str">
-        <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
-        <v>Sprint 1</v>
+      <c r="I9" s="6">
+        <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
+        <v>8</v>
       </c>
       <c r="J9" s="6"/>
     </row>
@@ -1446,13 +1452,13 @@
         <v>10</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>26</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>12</v>
@@ -1467,9 +1473,9 @@
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>8</v>
       </c>
-      <c r="I10" s="6" t="str">
-        <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
-        <v>Sprint 1</v>
+      <c r="I10" s="6">
+        <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
+        <v>8</v>
       </c>
       <c r="J10" s="6"/>
     </row>
@@ -1478,13 +1484,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>44</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>12</v>
@@ -1499,9 +1505,9 @@
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>5</v>
       </c>
-      <c r="I11" s="6" t="str">
-        <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
-        <v>Sprint 1</v>
+      <c r="I11" s="6">
+        <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
+        <v>5</v>
       </c>
       <c r="J11" s="6"/>
     </row>
@@ -1510,13 +1516,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>12</v>
@@ -1531,9 +1537,9 @@
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>5</v>
       </c>
-      <c r="I12" s="6" t="str">
-        <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
-        <v>Sprint 1</v>
+      <c r="I12" s="6">
+        <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
+        <v>5</v>
       </c>
       <c r="J12" s="6"/>
     </row>
@@ -1542,7 +1548,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>33</v>
@@ -1557,15 +1563,15 @@
         <v>2</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H13" s="6">
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>3</v>
       </c>
-      <c r="I13" s="6" t="str">
-        <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
-        <v>Sprint 1</v>
+      <c r="I13" s="6">
+        <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
+        <v>3</v>
       </c>
       <c r="J13" s="6" t="s">
         <v>14</v>
@@ -1576,7 +1582,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>33</v>
@@ -1591,15 +1597,15 @@
         <v>2</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H14" s="6">
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>3</v>
       </c>
-      <c r="I14" s="6" t="str">
-        <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
-        <v>Sprint 1</v>
+      <c r="I14" s="6">
+        <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
+        <v>3</v>
       </c>
       <c r="J14" s="6" t="s">
         <v>14</v>
@@ -1610,13 +1616,13 @@
         <v>10</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>12</v>
@@ -1631,12 +1637,12 @@
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>8</v>
       </c>
-      <c r="I15" s="6" t="str">
-        <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
-        <v>Sprint 1</v>
+      <c r="I15" s="6">
+        <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
+        <v>8</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1644,13 +1650,13 @@
         <v>10</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>12</v>
@@ -1665,12 +1671,12 @@
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>8</v>
       </c>
-      <c r="I16" s="6" t="str">
-        <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
-        <v>Sprint 1</v>
+      <c r="I16" s="6">
+        <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
+        <v>8</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1678,13 +1684,13 @@
         <v>10</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>12</v>
@@ -1699,12 +1705,12 @@
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>8</v>
       </c>
-      <c r="I17" s="6" t="str">
-        <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
-        <v>Sprint 1</v>
+      <c r="I17" s="6">
+        <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
+        <v>8</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1712,13 +1718,13 @@
         <v>10</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>27</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>12</v>
@@ -1733,9 +1739,9 @@
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>13</v>
       </c>
-      <c r="I18" s="6" t="str">
-        <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
-        <v>Sprint 1</v>
+      <c r="I18" s="6">
+        <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
+        <v>13</v>
       </c>
       <c r="J18" s="6"/>
     </row>
@@ -1744,7 +1750,7 @@
         <v>10</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>28</v>
@@ -1759,15 +1765,15 @@
         <v>2</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H19" s="6">
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>21</v>
       </c>
-      <c r="I19" s="6" t="str">
-        <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
-        <v>Sprint 1</v>
+      <c r="I19" s="6">
+        <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
+        <v>21</v>
       </c>
       <c r="J19" s="6"/>
     </row>
@@ -1776,7 +1782,7 @@
         <v>10</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>29</v>
@@ -1797,9 +1803,9 @@
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>8</v>
       </c>
-      <c r="I20" s="6" t="str">
-        <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
-        <v>Sprint 1</v>
+      <c r="I20" s="6">
+        <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
+        <v>8</v>
       </c>
       <c r="J20" s="6"/>
     </row>
@@ -1808,13 +1814,13 @@
         <v>10</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>39</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>12</v>
@@ -1829,21 +1835,21 @@
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>8</v>
       </c>
-      <c r="I21" s="6" t="str">
-        <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
-        <v>Sprint 1</v>
+      <c r="I21" s="6">
+        <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
+        <v>8</v>
       </c>
       <c r="J21" s="6"/>
     </row>
-    <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>69</v>
+        <v>101</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>78</v>
@@ -1855,96 +1861,94 @@
         <v>2</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="H22" s="6">
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
-        <v>5</v>
-      </c>
-      <c r="I22" s="6" t="str">
-        <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
-        <v>Sprint 1</v>
+        <v>8</v>
+      </c>
+      <c r="I22" s="6">
+        <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
+        <v>8</v>
       </c>
       <c r="J22" s="6"/>
     </row>
-    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>31</v>
       </c>
       <c r="F23" s="6">
+        <v>3</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H23" s="6">
+        <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
+        <v>13</v>
+      </c>
+      <c r="I23" s="6">
+        <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
+        <v>13</v>
+      </c>
+      <c r="J23" s="6"/>
+    </row>
+    <row r="24" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" s="6">
         <v>2</v>
       </c>
-      <c r="G23" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="H23" s="6">
-        <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
-        <v>8</v>
-      </c>
-      <c r="I23" s="6" t="str">
-        <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
-        <v>Sprint 1</v>
-      </c>
-      <c r="J23" s="6"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D24" s="7" t="s">
+      <c r="G24" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" s="6">
+        <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
+        <v>5</v>
+      </c>
+      <c r="I24" s="6">
+        <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
+        <v>5</v>
+      </c>
+      <c r="J24" s="6"/>
+    </row>
+    <row r="25" spans="1:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="E24" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="6">
-        <v>1</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="H24" s="6">
-        <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
-        <v>3</v>
-      </c>
-      <c r="I24" s="6" t="str">
-        <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
-        <v>Sprint 1</v>
-      </c>
-      <c r="J24" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>94</v>
-      </c>
       <c r="C25" s="7" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>31</v>
@@ -1953,62 +1957,64 @@
         <v>2</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="H25" s="6">
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>8</v>
       </c>
-      <c r="I25" s="6" t="str">
-        <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
-        <v>Sprint 1</v>
+      <c r="I25" s="6">
+        <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
+        <v>8</v>
       </c>
       <c r="J25" s="6"/>
     </row>
-    <row r="26" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F26" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>13</v>
+        <v>99</v>
       </c>
       <c r="H26" s="6">
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
-        <v>5</v>
-      </c>
-      <c r="I26" s="6" t="str">
-        <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
-        <v>Sprint 1</v>
+        <v>3</v>
+      </c>
+      <c r="I26" s="6">
+        <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
+        <v>3</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>98</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B27" s="6"/>
+        <v>76</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>92</v>
+      </c>
       <c r="C27" s="7" t="s">
-        <v>39</v>
+        <v>93</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>31</v>
@@ -2023,92 +2029,68 @@
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>8</v>
       </c>
-      <c r="I27" s="6" t="str">
-        <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
-        <v>Sprint 1</v>
+      <c r="I27" s="6">
+        <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
+        <v>8</v>
       </c>
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B28" s="6"/>
+        <v>76</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>94</v>
+      </c>
       <c r="C28" s="7" t="s">
-        <v>39</v>
+        <v>97</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="F28" s="6">
         <v>2</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="H28" s="6">
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
-        <v>8</v>
-      </c>
-      <c r="I28" s="6" t="str">
-        <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
-        <v>Sprint 1</v>
-      </c>
-      <c r="J28" s="6"/>
-    </row>
-    <row r="29" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>77</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="I28" s="6">
+        <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
+        <v>5</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
       <c r="B29" s="6"/>
-      <c r="C29" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F29" s="6">
-        <v>3</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="H29" s="6">
-        <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
-        <v>13</v>
-      </c>
-      <c r="I29" s="6" t="str">
-        <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
-        <v>Sprint 1</v>
-      </c>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
       <c r="J29" s="6"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>77</v>
-      </c>
+      <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
-      <c r="G30" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H30" s="6">
-        <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
-        <v>5</v>
-      </c>
-      <c r="I30" s="6" t="str">
-        <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
-        <v>Sprint 1</v>
-      </c>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
       <c r="J30" s="6"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2119,14 +2101,8 @@
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
-      <c r="H31" s="6" t="str">
-        <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
-        <v/>
-      </c>
-      <c r="I31" s="6" t="str">
-        <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
-        <v/>
-      </c>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
       <c r="J31" s="6"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -2137,15 +2113,21 @@
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
-      <c r="H32" s="6" t="str">
-        <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
-        <v/>
-      </c>
-      <c r="I32" s="6" t="str">
-        <f>IF(Tabela1[[#This Row],[Categoria]] = "Funcional", "Sprint 1",IF(Tabela1[[#This Row],[Categoria]] = "Não funcional","Sprint 1",""))</f>
-        <v/>
-      </c>
+      <c r="H32" s="17"/>
+      <c r="I32" s="6"/>
       <c r="J32" s="6"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Nova paleta de cores, adição da função de cadastro e login
</commit_message>
<xml_diff>
--- a/Documentação/Product backlogs.xlsx
+++ b/Documentação/Product backlogs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/samuel_barros_sptech_school/Documents/Documentos/Algoritmo/Aula 3/SPtech/Projeto-pessoal/Documentação/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="496" documentId="11_AD4D361C20488DEA4E38A0F40C5A5BD05ADEDD78" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E700C25-CE6B-4BA5-BB1D-BD97477A45A8}"/>
+  <xr:revisionPtr revIDLastSave="497" documentId="11_AD4D361C20488DEA4E38A0F40C5A5BD05ADEDD78" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B4BE9A8-C07C-4110-B8C0-030C7685A2F8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="103">
   <si>
     <t>Categoria</t>
   </si>
@@ -519,7 +519,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -569,9 +569,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,7 +587,6 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -606,6 +602,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -814,10 +811,10 @@
     <tableColumn id="8" xr3:uid="{E55713D6-BEF4-4E2B-A894-0176E4987129}" name="Tam(#)" dataDxfId="2">
       <calculatedColumnFormula>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{53EA01A0-EC01-402F-BA49-1E4B7904D7B8}" name="Sprint" dataDxfId="0">
+    <tableColumn id="9" xr3:uid="{53EA01A0-EC01-402F-BA49-1E4B7904D7B8}" name="Sprint" dataDxfId="1">
       <calculatedColumnFormula>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{D68286FD-EF48-4F7F-B2D3-35D2D998121E}" name="Sprint semanal" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{D68286FD-EF48-4F7F-B2D3-35D2D998121E}" name="Sprint semanal" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1088,8 +1085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,7 +1331,7 @@
       </c>
       <c r="M6" s="10">
         <f>SUMIF(J:J,"Semana 3",H:H)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -2033,7 +2030,9 @@
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>8</v>
       </c>
-      <c r="J27" s="6"/>
+      <c r="J27" s="6" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
@@ -2113,7 +2112,7 @@
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
-      <c r="H32" s="17"/>
+      <c r="H32" s="6"/>
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
     </row>

</xml_diff>

<commit_message>
Novo loyout das curtidas, sistema sanduiche dos comenatarios
</commit_message>
<xml_diff>
--- a/Documentação/Product backlogs.xlsx
+++ b/Documentação/Product backlogs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/samuel_barros_sptech_school/Documents/Documentos/Algoritmo/Aula 3/SPtech/Projeto-pessoal/Documentação/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="497" documentId="11_AD4D361C20488DEA4E38A0F40C5A5BD05ADEDD78" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B4BE9A8-C07C-4110-B8C0-030C7685A2F8}"/>
+  <xr:revisionPtr revIDLastSave="513" documentId="11_AD4D361C20488DEA4E38A0F40C5A5BD05ADEDD78" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA469D43-0D33-464E-8350-3F4842A5014B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="103">
   <si>
     <t>Categoria</t>
   </si>
@@ -351,7 +351,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -378,6 +378,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -519,7 +526,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -567,6 +574,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1085,8 +1095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="C44" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1205,7 +1215,9 @@
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>8</v>
       </c>
-      <c r="J3" s="6"/>
+      <c r="J3" s="6" t="s">
+        <v>83</v>
+      </c>
       <c r="L3" s="9" t="s">
         <v>80</v>
       </c>
@@ -1292,7 +1304,7 @@
       </c>
       <c r="M5" s="10">
         <f>SUMIF(J:J,"Semana 2",H:H)</f>
-        <v>24</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -1325,13 +1337,15 @@
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>8</v>
       </c>
-      <c r="J6" s="6"/>
+      <c r="J6" s="6" t="s">
+        <v>82</v>
+      </c>
       <c r="L6" s="9" t="s">
         <v>83</v>
       </c>
       <c r="M6" s="10">
         <f>SUMIF(J:J,"Semana 3",H:H)</f>
-        <v>8</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1364,13 +1378,15 @@
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>8</v>
       </c>
-      <c r="J7" s="6"/>
+      <c r="J7" s="6" t="s">
+        <v>83</v>
+      </c>
       <c r="L7" s="11" t="s">
         <v>84</v>
       </c>
       <c r="M7" s="12">
         <f>SUMIF(J:J,"Semana 4",H:H)</f>
-        <v>0</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -1403,7 +1419,9 @@
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>8</v>
       </c>
-      <c r="J8" s="6"/>
+      <c r="J8" s="6" t="s">
+        <v>83</v>
+      </c>
       <c r="L8" s="13" t="s">
         <v>86</v>
       </c>
@@ -1442,7 +1460,9 @@
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>8</v>
       </c>
-      <c r="J9" s="6"/>
+      <c r="J9" s="6" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
@@ -1474,7 +1494,9 @@
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>8</v>
       </c>
-      <c r="J10" s="6"/>
+      <c r="J10" s="6" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
@@ -1506,7 +1528,9 @@
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>5</v>
       </c>
-      <c r="J11" s="6"/>
+      <c r="J11" s="6" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
@@ -1538,7 +1562,9 @@
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>5</v>
       </c>
-      <c r="J12" s="6"/>
+      <c r="J12" s="6" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
@@ -1740,7 +1766,9 @@
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>13</v>
       </c>
-      <c r="J18" s="6"/>
+      <c r="J18" s="6" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
@@ -1772,7 +1800,9 @@
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>21</v>
       </c>
-      <c r="J19" s="6"/>
+      <c r="J19" s="6" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
@@ -1804,7 +1834,9 @@
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>8</v>
       </c>
-      <c r="J20" s="6"/>
+      <c r="J20" s="6" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="21" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
@@ -1836,7 +1868,9 @@
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>8</v>
       </c>
-      <c r="J21" s="6"/>
+      <c r="J21" s="6" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
@@ -1868,7 +1902,9 @@
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>8</v>
       </c>
-      <c r="J22" s="6"/>
+      <c r="J22" s="6" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
@@ -1900,7 +1936,9 @@
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>13</v>
       </c>
-      <c r="J23" s="6"/>
+      <c r="J23" s="6" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="24" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
@@ -1932,7 +1970,7 @@
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>5</v>
       </c>
-      <c r="J24" s="6"/>
+      <c r="J24" s="17"/>
     </row>
     <row r="25" spans="1:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
@@ -1964,7 +2002,9 @@
         <f>IF(Tabela1[[#This Row],[Tamanho]] = "Muito Pequeno", 3,IF(Tabela1[[#This Row],[Tamanho]] = "Pequeno", 5,IF(Tabela1[[#This Row],[Tamanho]] = "Médio", 8,IF(Tabela1[[#This Row],[Tamanho]] = "Grande", 13,IF(Tabela1[[#This Row],[Tamanho]] = "Muito Grande", 21,"")))))</f>
         <v>8</v>
       </c>
-      <c r="J25" s="6"/>
+      <c r="J25" s="6" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">

</xml_diff>